<commit_message>
Checkpoint because of scripts that will be used to generate c files
</commit_message>
<xml_diff>
--- a/calibration_data/0045001D334B501920313046_cal_graph.xlsx
+++ b/calibration_data/0045001D334B501920313046_cal_graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\forge\outdoor-monitor\lm_script\calibration_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D5E929E-800D-4531-B0DB-5726BE876A19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{483ADB86-CBA8-4F47-A57A-28CDEB95BE0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="510" windowWidth="25440" windowHeight="15390"/>
   </bookViews>
@@ -573,6 +573,35 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sensor</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Calibration - Apparent issue at 23.5</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2055,8 +2084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B52"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="T43" sqref="T43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>